<commit_message>
Update the tracking list
</commit_message>
<xml_diff>
--- a/Team Ramp-up Tracking.xlsx
+++ b/Team Ramp-up Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAP\SAP_Projects\SME\SME WIP\Ramp-up Plan\Status Tracking\Team-Ramp-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC9BDB8-AA86-4ECF-B4AE-EA64ED32DA83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0A1CCF-97BD-42E8-ABA2-0F009FE0D22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2311,10 +2311,10 @@
   <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2327,7 +2327,7 @@
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.1328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.46484375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1328125" style="1" customWidth="1"/>
     <col min="11" max="14" width="18.1328125" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.86328125" style="1" customWidth="1"/>
     <col min="16" max="18" width="18.1328125" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
Merge the update functions
</commit_message>
<xml_diff>
--- a/Team Ramp-up Tracking.xlsx
+++ b/Team Ramp-up Tracking.xlsx
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -113,6 +113,9 @@
     </font>
     <font>
       <color rgb="00000000"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="10">
@@ -312,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -436,6 +439,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="7" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="7" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="8" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="8" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="7" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2083,7 +2098,7 @@
         </is>
       </c>
       <c r="J12" s="25" t="n"/>
-      <c r="K12" s="33" t="inlineStr">
+      <c r="K12" s="41" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -2159,7 +2174,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K13" s="29" t="inlineStr">
+      <c r="K13" s="42" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -2247,7 +2262,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="K14" s="33" t="inlineStr">
+      <c r="K14" s="41" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -2335,7 +2350,7 @@
         </is>
       </c>
       <c r="J15" s="27" t="n"/>
-      <c r="K15" s="34" t="inlineStr">
+      <c r="K15" s="43" t="inlineStr">
         <is>
           <t>90</t>
         </is>
@@ -2403,7 +2418,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K16" s="33" t="inlineStr">
+      <c r="K16" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -2727,7 +2742,7 @@
           <t>50</t>
         </is>
       </c>
-      <c r="K21" s="34" t="inlineStr">
+      <c r="K21" s="43" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -2867,7 +2882,7 @@
         </is>
       </c>
       <c r="J23" s="27" t="n"/>
-      <c r="K23" s="34" t="inlineStr">
+      <c r="K23" s="43" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -2947,7 +2962,7 @@
         </is>
       </c>
       <c r="J24" s="25" t="n"/>
-      <c r="K24" s="33" t="inlineStr">
+      <c r="K24" s="41" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -3071,7 +3086,7 @@
         </is>
       </c>
       <c r="J26" s="25" t="n"/>
-      <c r="K26" s="33" t="inlineStr">
+      <c r="K26" s="41" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -3219,7 +3234,7 @@
         </is>
       </c>
       <c r="J28" s="25" t="n"/>
-      <c r="K28" s="33" t="inlineStr">
+      <c r="K28" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -3291,7 +3306,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K29" s="34" t="inlineStr">
+      <c r="K29" s="43" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -3355,7 +3370,7 @@
         </is>
       </c>
       <c r="J30" s="25" t="n"/>
-      <c r="K30" s="33" t="inlineStr">
+      <c r="K30" s="41" t="inlineStr">
         <is>
           <t>90</t>
         </is>
@@ -3503,7 +3518,7 @@
         </is>
       </c>
       <c r="J32" s="25" t="n"/>
-      <c r="K32" s="33" t="inlineStr">
+      <c r="K32" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -3567,7 +3582,7 @@
         </is>
       </c>
       <c r="J33" s="27" t="n"/>
-      <c r="K33" s="34" t="inlineStr">
+      <c r="K33" s="43" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -3739,7 +3754,7 @@
         </is>
       </c>
       <c r="J36" s="25" t="n"/>
-      <c r="K36" s="33" t="inlineStr">
+      <c r="K36" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -3887,7 +3902,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="K38" s="33" t="inlineStr">
+      <c r="K38" s="41" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -4163,7 +4178,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K42" s="33" t="inlineStr">
+      <c r="K42" s="41" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -4235,7 +4250,7 @@
           <t>80</t>
         </is>
       </c>
-      <c r="K43" s="34" t="inlineStr">
+      <c r="K43" s="43" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -4303,7 +4318,7 @@
         </is>
       </c>
       <c r="J44" s="25" t="n"/>
-      <c r="K44" s="33" t="inlineStr">
+      <c r="K44" s="41" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -4443,7 +4458,7 @@
         </is>
       </c>
       <c r="J46" s="25" t="n"/>
-      <c r="K46" s="33" t="inlineStr">
+      <c r="K46" s="41" t="inlineStr">
         <is>
           <t>30</t>
         </is>
@@ -4639,7 +4654,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="K49" s="34" t="inlineStr">
+      <c r="K49" s="43" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -4847,7 +4862,7 @@
         </is>
       </c>
       <c r="J52" s="25" t="n"/>
-      <c r="K52" s="33" t="inlineStr">
+      <c r="K52" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -4919,7 +4934,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="K53" s="34" t="inlineStr">
+      <c r="K53" s="43" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -4999,7 +5014,7 @@
         </is>
       </c>
       <c r="J54" s="25" t="n"/>
-      <c r="K54" s="33" t="inlineStr">
+      <c r="K54" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -5139,7 +5154,7 @@
         </is>
       </c>
       <c r="J56" s="25" t="n"/>
-      <c r="K56" s="33" t="inlineStr">
+      <c r="K56" s="41" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -5271,7 +5286,7 @@
         </is>
       </c>
       <c r="J58" s="25" t="n"/>
-      <c r="K58" s="33" t="inlineStr">
+      <c r="K58" s="41" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -5335,7 +5350,7 @@
         </is>
       </c>
       <c r="J59" s="27" t="n"/>
-      <c r="K59" s="34" t="inlineStr">
+      <c r="K59" s="43" t="inlineStr">
         <is>
           <t>50</t>
         </is>
@@ -5479,7 +5494,7 @@
           <t>60</t>
         </is>
       </c>
-      <c r="K61" s="34" t="inlineStr">
+      <c r="K61" s="43" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -5603,7 +5618,7 @@
           <t>90</t>
         </is>
       </c>
-      <c r="K63" s="34" t="inlineStr">
+      <c r="K63" s="43" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -5683,7 +5698,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K64" s="34" t="inlineStr">
+      <c r="K64" s="43" t="inlineStr">
         <is>
           <t>60</t>
         </is>
@@ -5913,7 +5928,7 @@
           <t>20</t>
         </is>
       </c>
-      <c r="K67" s="29" t="inlineStr">
+      <c r="K67" s="42" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -5993,7 +6008,7 @@
           <t>40</t>
         </is>
       </c>
-      <c r="K68" s="31" t="inlineStr">
+      <c r="K68" s="44" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -6233,7 +6248,7 @@
           <t>50</t>
         </is>
       </c>
-      <c r="K71" s="29" t="inlineStr">
+      <c r="K71" s="42" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -6713,7 +6728,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K77" s="29" t="inlineStr">
+      <c r="K77" s="42" t="inlineStr">
         <is>
           <t>70</t>
         </is>
@@ -6793,7 +6808,7 @@
           <t>30</t>
         </is>
       </c>
-      <c r="K78" s="31" t="inlineStr">
+      <c r="K78" s="44" t="inlineStr">
         <is>
           <t>80</t>
         </is>
@@ -6873,7 +6888,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K79" s="29" t="inlineStr">
+      <c r="K79" s="42" t="inlineStr">
         <is>
           <t>60</t>
         </is>
@@ -6953,7 +6968,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="K80" s="31" t="inlineStr">
+      <c r="K80" s="44" t="inlineStr">
         <is>
           <t>50</t>
         </is>

</xml_diff>

<commit_message>
Add the function to create summary list
</commit_message>
<xml_diff>
--- a/Team Ramp-up Tracking.xlsx
+++ b/Team Ramp-up Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap.sharepoint.com/teams/X4PlatformCNTeamRamp-up/Shared Documents/General/Tracking List/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SAP\SAP_Projects\SME\SME WIP\Ramp-up Plan\Status Tracking\Team-Ramp-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="5_{59082984-9A5F-49CC-B90D-3BA22979DD94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{ED1C041B-DC95-4D99-A20E-C5197072BB8B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5D7EC3-3FBE-4936-8EC9-8EEDDBFD1FDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3022" yWindow="442" windowWidth="15068" windowHeight="9353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="385">
   <si>
     <t>Employee_ID</t>
   </si>
@@ -232,48 +232,48 @@
     <t>X*</t>
   </si>
   <si>
+    <t>I029546</t>
+  </si>
+  <si>
+    <t>Zhang Meng</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>Meng</t>
+  </si>
+  <si>
+    <t>Yuedong Chen</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>I031427</t>
+  </si>
+  <si>
+    <t>Ingrid Wang</t>
+  </si>
+  <si>
+    <t>Wang</t>
+  </si>
+  <si>
+    <t>Xu</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Quality Expert</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
-    <t>I029546</t>
-  </si>
-  <si>
-    <t>Zhang Meng</t>
-  </si>
-  <si>
-    <t>Zhang</t>
-  </si>
-  <si>
-    <t>Meng</t>
-  </si>
-  <si>
-    <t>Yuedong Chen</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>I031427</t>
-  </si>
-  <si>
-    <t>Ingrid Wang</t>
-  </si>
-  <si>
-    <t>Wang</t>
-  </si>
-  <si>
-    <t>Xu</t>
-  </si>
-  <si>
-    <t>Ingrid</t>
-  </si>
-  <si>
-    <t>Quality Expert</t>
-  </si>
-  <si>
-    <t>QS</t>
-  </si>
-  <si>
     <t>I052065</t>
   </si>
   <si>
@@ -406,45 +406,48 @@
     <t>Extra</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>I015290</t>
+  </si>
+  <si>
+    <t>Kevin Zhang</t>
+  </si>
+  <si>
+    <t>Zhonghua</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Meng Zhang</t>
+  </si>
+  <si>
+    <t>I065754</t>
+  </si>
+  <si>
+    <t>Ivan Sheng</t>
+  </si>
+  <si>
+    <t>Sheng</t>
+  </si>
+  <si>
+    <t>Yiwei</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Senior Developer</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
-    <t>I015290</t>
-  </si>
-  <si>
-    <t>Kevin Zhang</t>
-  </si>
-  <si>
-    <t>Zhonghua</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Meng Zhang</t>
-  </si>
-  <si>
-    <t>I065754</t>
-  </si>
-  <si>
-    <t>Ivan Sheng</t>
-  </si>
-  <si>
-    <t>Sheng</t>
-  </si>
-  <si>
-    <t>Yiwei</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Senior Developer</t>
-  </si>
-  <si>
-    <t>JD</t>
-  </si>
-  <si>
     <t>I068662</t>
   </si>
   <si>
@@ -535,369 +538,366 @@
     <t>Xiongjun</t>
   </si>
   <si>
+    <t>I075064</t>
+  </si>
+  <si>
+    <t>Abby Cui</t>
+  </si>
+  <si>
+    <t>Cui</t>
+  </si>
+  <si>
+    <t>Hongxia</t>
+  </si>
+  <si>
+    <t>Abby</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>I075066</t>
+  </si>
+  <si>
+    <t>Liu Ying</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>Ying</t>
+  </si>
+  <si>
+    <t>I076353</t>
+  </si>
+  <si>
+    <t>Cham Xu</t>
+  </si>
+  <si>
+    <t>Qian</t>
+  </si>
+  <si>
+    <t>Cham</t>
+  </si>
+  <si>
+    <t>I077230</t>
+  </si>
+  <si>
+    <t>Gordon Liu</t>
+  </si>
+  <si>
+    <t>Jinguo</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>I300463</t>
+  </si>
+  <si>
+    <t>Zachary Li</t>
+  </si>
+  <si>
+    <t>Yixuan</t>
+  </si>
+  <si>
+    <t>Zachary</t>
+  </si>
+  <si>
+    <t>I300974</t>
+  </si>
+  <si>
+    <t>Helene Chen</t>
+  </si>
+  <si>
+    <t>Xiaoyi</t>
+  </si>
+  <si>
+    <t>Helene</t>
+  </si>
+  <si>
+    <t>Senior User Experience Design Specialist</t>
+  </si>
+  <si>
+    <t>I306429</t>
+  </si>
+  <si>
+    <t>Telford Zhao</t>
+  </si>
+  <si>
+    <t>Zhao</t>
+  </si>
+  <si>
+    <t>Tiefu</t>
+  </si>
+  <si>
+    <t>Telford</t>
+  </si>
+  <si>
+    <t>I308164</t>
+  </si>
+  <si>
+    <t>Roy Shao</t>
+  </si>
+  <si>
+    <t>Shao</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>Quality Specialist</t>
+  </si>
+  <si>
+    <t>I308454</t>
+  </si>
+  <si>
+    <t>Cao Li</t>
+  </si>
+  <si>
+    <t>Cao</t>
+  </si>
+  <si>
+    <t>I309938</t>
+  </si>
+  <si>
+    <t>Alex Li</t>
+  </si>
+  <si>
+    <t>Zhen</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>I313530</t>
+  </si>
+  <si>
+    <t>Zhao Luyi</t>
+  </si>
+  <si>
+    <t>Luyi</t>
+  </si>
+  <si>
+    <t>I322858</t>
+  </si>
+  <si>
+    <t>Li Linju</t>
+  </si>
+  <si>
+    <t>Linju</t>
+  </si>
+  <si>
+    <t>I323866</t>
+  </si>
+  <si>
+    <t>Chen Qi</t>
+  </si>
+  <si>
+    <t>Qi</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>I324508</t>
+  </si>
+  <si>
+    <t>Felix Huang</t>
+  </si>
+  <si>
+    <t>Zehao</t>
+  </si>
+  <si>
+    <t>Felix</t>
+  </si>
+  <si>
+    <t>I324714</t>
+  </si>
+  <si>
+    <t>Meng Di</t>
+  </si>
+  <si>
+    <t>Di</t>
+  </si>
+  <si>
+    <t>User Assistance Developer Associate</t>
+  </si>
+  <si>
+    <t>I326827</t>
+  </si>
+  <si>
+    <t>Jeremy Wu</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>Zhenhao</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
-    <t>I075064</t>
-  </si>
-  <si>
-    <t>Abby Cui</t>
-  </si>
-  <si>
-    <t>Cui</t>
-  </si>
-  <si>
-    <t>Hongxia</t>
-  </si>
-  <si>
-    <t>Abby</t>
-  </si>
-  <si>
-    <t>SM</t>
-  </si>
-  <si>
-    <t>I075066</t>
-  </si>
-  <si>
-    <t>Liu Ying</t>
-  </si>
-  <si>
-    <t>Liu</t>
-  </si>
-  <si>
-    <t>Ying</t>
-  </si>
-  <si>
-    <t>I076353</t>
-  </si>
-  <si>
-    <t>Cham Xu</t>
-  </si>
-  <si>
-    <t>Qian</t>
-  </si>
-  <si>
-    <t>Cham</t>
-  </si>
-  <si>
-    <t>I077230</t>
-  </si>
-  <si>
-    <t>Gordon Liu</t>
-  </si>
-  <si>
-    <t>Jinguo</t>
-  </si>
-  <si>
-    <t>Gordon</t>
-  </si>
-  <si>
-    <t>I300463</t>
-  </si>
-  <si>
-    <t>Zachary Li</t>
-  </si>
-  <si>
-    <t>Yixuan</t>
-  </si>
-  <si>
-    <t>Zachary</t>
+    <t>I327506</t>
+  </si>
+  <si>
+    <t>Adam Wang</t>
+  </si>
+  <si>
+    <t>Kechen</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Developer Associate</t>
+  </si>
+  <si>
+    <t>I329682</t>
+  </si>
+  <si>
+    <t>Jerry Liu</t>
+  </si>
+  <si>
+    <t>Jia</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>I338782</t>
+  </si>
+  <si>
+    <t>William Ye</t>
+  </si>
+  <si>
+    <t>Ye</t>
+  </si>
+  <si>
+    <t>Shengren</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>I339354</t>
+  </si>
+  <si>
+    <t>Andy Feng</t>
+  </si>
+  <si>
+    <t>Feng</t>
+  </si>
+  <si>
+    <t>Jiawei</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>User Experience Design Specialist</t>
+  </si>
+  <si>
+    <t>I340146</t>
+  </si>
+  <si>
+    <t>Thomas Hu</t>
+  </si>
+  <si>
+    <t>Hu</t>
+  </si>
+  <si>
+    <t>Ming</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>I342835</t>
+  </si>
+  <si>
+    <t>Lucas Liu</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>I052252</t>
+  </si>
+  <si>
+    <t>Buffon Sun</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Bufeng</t>
+  </si>
+  <si>
+    <t>Buffon</t>
+  </si>
+  <si>
+    <t>I349262</t>
+  </si>
+  <si>
+    <t>Dong Liyan</t>
+  </si>
+  <si>
+    <t>Dong</t>
+  </si>
+  <si>
+    <t>Liyan</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>I321714</t>
+  </si>
+  <si>
+    <t>Zhou Kaiyuan</t>
+  </si>
+  <si>
+    <t>Zhou</t>
+  </si>
+  <si>
+    <t>Kaiyuan</t>
+  </si>
+  <si>
+    <t>I518769</t>
+  </si>
+  <si>
+    <t>Allen Xiong</t>
+  </si>
+  <si>
+    <t>Xiong</t>
+  </si>
+  <si>
+    <t>Jie</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>I039142</t>
+  </si>
+  <si>
+    <t>Trevor Zhang</t>
+  </si>
+  <si>
+    <t>Tonghe</t>
+  </si>
+  <si>
+    <t>Trevor</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>I300974</t>
-  </si>
-  <si>
-    <t>Helene Chen</t>
-  </si>
-  <si>
-    <t>Xiaoyi</t>
-  </si>
-  <si>
-    <t>Helene</t>
-  </si>
-  <si>
-    <t>Senior User Experience Design Specialist</t>
-  </si>
-  <si>
-    <t>I306429</t>
-  </si>
-  <si>
-    <t>Telford Zhao</t>
-  </si>
-  <si>
-    <t>Zhao</t>
-  </si>
-  <si>
-    <t>Tiefu</t>
-  </si>
-  <si>
-    <t>Telford</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>I308164</t>
-  </si>
-  <si>
-    <t>Roy Shao</t>
-  </si>
-  <si>
-    <t>Shao</t>
-  </si>
-  <si>
-    <t>Roy</t>
-  </si>
-  <si>
-    <t>Quality Specialist</t>
-  </si>
-  <si>
-    <t>I308454</t>
-  </si>
-  <si>
-    <t>Cao Li</t>
-  </si>
-  <si>
-    <t>Cao</t>
-  </si>
-  <si>
-    <t>I309938</t>
-  </si>
-  <si>
-    <t>Alex Li</t>
-  </si>
-  <si>
-    <t>Zhen</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>I313530</t>
-  </si>
-  <si>
-    <t>Zhao Luyi</t>
-  </si>
-  <si>
-    <t>Luyi</t>
-  </si>
-  <si>
-    <t>I322858</t>
-  </si>
-  <si>
-    <t>Li Linju</t>
-  </si>
-  <si>
-    <t>Linju</t>
-  </si>
-  <si>
-    <t>I323866</t>
-  </si>
-  <si>
-    <t>Chen Qi</t>
-  </si>
-  <si>
-    <t>Qi</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>I324508</t>
-  </si>
-  <si>
-    <t>Felix Huang</t>
-  </si>
-  <si>
-    <t>Zehao</t>
-  </si>
-  <si>
-    <t>Felix</t>
-  </si>
-  <si>
-    <t>I324714</t>
-  </si>
-  <si>
-    <t>Meng Di</t>
-  </si>
-  <si>
-    <t>Di</t>
-  </si>
-  <si>
-    <t>User Assistance Developer Associate</t>
-  </si>
-  <si>
-    <t>I326827</t>
-  </si>
-  <si>
-    <t>Jeremy Wu</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t>Zhenhao</t>
-  </si>
-  <si>
-    <t>Jeremy</t>
-  </si>
-  <si>
-    <t>I327506</t>
-  </si>
-  <si>
-    <t>Adam Wang</t>
-  </si>
-  <si>
-    <t>Kechen</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Developer Associate</t>
-  </si>
-  <si>
-    <t>I329682</t>
-  </si>
-  <si>
-    <t>Jerry Liu</t>
-  </si>
-  <si>
-    <t>Jia</t>
-  </si>
-  <si>
-    <t>Jerry</t>
-  </si>
-  <si>
-    <t>I338782</t>
-  </si>
-  <si>
-    <t>William Ye</t>
-  </si>
-  <si>
-    <t>Ye</t>
-  </si>
-  <si>
-    <t>Shengren</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>I339354</t>
-  </si>
-  <si>
-    <t>Andy Feng</t>
-  </si>
-  <si>
-    <t>Feng</t>
-  </si>
-  <si>
-    <t>Jiawei</t>
-  </si>
-  <si>
-    <t>Andy</t>
-  </si>
-  <si>
-    <t>User Experience Design Specialist</t>
-  </si>
-  <si>
-    <t>I340146</t>
-  </si>
-  <si>
-    <t>Thomas Hu</t>
-  </si>
-  <si>
-    <t>Hu</t>
-  </si>
-  <si>
-    <t>Ming</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>I342835</t>
-  </si>
-  <si>
-    <t>Lucas Liu</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>I052252</t>
-  </si>
-  <si>
-    <t>Buffon Sun</t>
-  </si>
-  <si>
-    <t>Sun</t>
-  </si>
-  <si>
-    <t>Bufeng</t>
-  </si>
-  <si>
-    <t>Buffon</t>
-  </si>
-  <si>
-    <t>I349262</t>
-  </si>
-  <si>
-    <t>Dong Liyan</t>
-  </si>
-  <si>
-    <t>Dong</t>
-  </si>
-  <si>
-    <t>Liyan</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>I321714</t>
-  </si>
-  <si>
-    <t>Zhou Kaiyuan</t>
-  </si>
-  <si>
-    <t>Zhou</t>
-  </si>
-  <si>
-    <t>Kaiyuan</t>
-  </si>
-  <si>
-    <t>I518769</t>
-  </si>
-  <si>
-    <t>Allen Xiong</t>
-  </si>
-  <si>
-    <t>Xiong</t>
-  </si>
-  <si>
-    <t>Jie</t>
-  </si>
-  <si>
-    <t>Allen</t>
-  </si>
-  <si>
-    <t>I039142</t>
-  </si>
-  <si>
-    <t>Trevor Zhang</t>
-  </si>
-  <si>
-    <t>Tonghe</t>
-  </si>
-  <si>
-    <t>Trevor</t>
-  </si>
-  <si>
     <t>I055660</t>
   </si>
   <si>
@@ -1157,6 +1157,9 @@
   </si>
   <si>
     <t>Ray</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>I070635</t>
@@ -1253,7 +1256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1284,6 +1287,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1478,7 +1486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1575,9 +1583,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1597,6 +1602,33 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2388,10 +2420,10 @@
   <dimension ref="A1:S89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2404,61 +2436,61 @@
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="3" customWidth="1"/>
     <col min="9" max="19" width="12.86328125" style="1" customWidth="1"/>
-    <col min="20" max="22" width="9.1328125" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1328125" style="1"/>
+    <col min="20" max="23" width="9.1328125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="40">
+      <c r="I1" s="48">
         <v>43678</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="40">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="48">
         <v>43709</v>
       </c>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="42"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="50"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="32" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="39" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -2592,12 +2624,14 @@
       <c r="N4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="P4" s="16" t="s">
         <v>44</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>44</v>
@@ -2608,20 +2642,20 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>42</v>
@@ -2630,7 +2664,7 @@
         <v>43</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>44</v>
@@ -2665,36 +2699,36 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="17" t="s">
-        <v>58</v>
-      </c>
       <c r="I6" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="21"/>
@@ -2703,7 +2737,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="21"/>
       <c r="S6" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
@@ -2714,14 +2748,14 @@
         <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>42</v>
@@ -2778,7 +2812,7 @@
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>66</v>
@@ -2835,7 +2869,7 @@
         <v>73</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>74</v>
@@ -2844,7 +2878,7 @@
         <v>75</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="23"/>
@@ -2852,7 +2886,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P9" s="23"/>
       <c r="Q9" s="18"/>
@@ -2876,7 +2910,7 @@
         <v>80</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>81</v>
@@ -2913,7 +2947,7 @@
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>81</v>
@@ -2922,7 +2956,7 @@
         <v>82</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="23"/>
@@ -2943,7 +2977,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>89</v>
@@ -2952,7 +2986,7 @@
         <v>90</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>91</v>
@@ -2967,25 +3001,25 @@
       <c r="K12" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="38" t="s">
+      <c r="L12" s="37" t="s">
         <v>94</v>
       </c>
       <c r="M12" s="16"/>
-      <c r="N12" s="21" t="s">
-        <v>45</v>
+      <c r="N12" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="16"/>
       <c r="R12" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S12" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -3003,42 +3037,44 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="19" t="s">
         <v>67</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="34" t="s">
+      <c r="L13" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="M13" s="34" t="s">
-        <v>51</v>
+      <c r="M13" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="O13" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="P13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -3058,7 +3094,7 @@
         <v>102</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="17" t="s">
@@ -3067,33 +3103,35 @@
       <c r="I14" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="L14" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="M14" s="33" t="s">
+      <c r="M14" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="N14" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="O14" s="21"/>
+      <c r="N14" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>44</v>
+      </c>
       <c r="P14" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q14" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S14" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -3104,7 +3142,7 @@
         <v>105</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>106</v>
@@ -3132,12 +3170,12 @@
       <c r="M15" s="18"/>
       <c r="N15" s="23"/>
       <c r="O15" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P15" s="23"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S15" s="23"/>
     </row>
@@ -3169,42 +3207,42 @@
       <c r="I16" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="36" t="s">
+      <c r="J16" s="35" t="s">
         <v>93</v>
       </c>
       <c r="K16" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>45</v>
+      <c r="L16" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="21"/>
       <c r="O16" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P16" s="21"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S16" s="21"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>108</v>
@@ -3220,36 +3258,36 @@
       </c>
       <c r="J17" s="18"/>
       <c r="K17" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L17" s="23"/>
       <c r="M17" s="18"/>
       <c r="N17" s="23"/>
       <c r="O17" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P17" s="23"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S17" s="23"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>108</v>
@@ -3267,7 +3305,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="21"/>
       <c r="O18" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P18" s="21"/>
       <c r="Q18" s="16"/>
@@ -3276,16 +3314,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="18" t="s">
@@ -3295,51 +3333,51 @@
         <v>66</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>68</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L19" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19" s="18"/>
-      <c r="N19" s="23" t="s">
-        <v>45</v>
+      <c r="N19" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P19" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q19" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R19" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S19" s="23"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>108</v>
@@ -3351,42 +3389,42 @@
         <v>82</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="21" t="s">
-        <v>45</v>
+      <c r="N20" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q20" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>108</v>
@@ -3395,48 +3433,48 @@
         <v>91</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L21" s="39" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>116</v>
       </c>
       <c r="M21" s="18"/>
       <c r="N21" s="23"/>
       <c r="O21" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P21" s="23"/>
       <c r="Q21" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S21" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="16" t="s">
@@ -3446,48 +3484,48 @@
         <v>114</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="L22" s="40" t="s">
+        <v>50</v>
       </c>
       <c r="M22" s="16"/>
       <c r="N22" s="21"/>
       <c r="O22" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P22" s="21"/>
       <c r="Q22" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R22" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S22" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="18" t="s">
@@ -3500,31 +3538,31 @@
         <v>82</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J23" s="18"/>
-      <c r="K23" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>146</v>
+      <c r="K23" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="L23" s="41" t="s">
+        <v>93</v>
       </c>
       <c r="M23" s="18"/>
-      <c r="N23" s="23" t="s">
-        <v>45</v>
+      <c r="N23" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P23" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q23" s="18"/>
       <c r="R23" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S23" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -3553,28 +3591,28 @@
         <v>152</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="L24" s="38" t="s">
+      <c r="L24" s="37" t="s">
         <v>93</v>
       </c>
       <c r="M24" s="16"/>
-      <c r="N24" s="21" t="s">
-        <v>45</v>
+      <c r="N24" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q24" s="16"/>
       <c r="R24" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S24" s="21"/>
     </row>
@@ -3608,7 +3646,7 @@
       <c r="M25" s="18"/>
       <c r="N25" s="23"/>
       <c r="O25" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P25" s="23"/>
       <c r="Q25" s="18"/>
@@ -3623,7 +3661,7 @@
         <v>158</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>159</v>
@@ -3641,26 +3679,26 @@
         <v>82</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J26" s="16"/>
-      <c r="K26" s="24" t="s">
-        <v>103</v>
+      <c r="K26" s="40" t="s">
+        <v>94</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N26" s="21"/>
       <c r="O26" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P26" s="21"/>
       <c r="Q26" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R26" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S26" s="21"/>
     </row>
@@ -3694,24 +3732,24 @@
       </c>
       <c r="J27" s="18"/>
       <c r="K27" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L27" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="L27" s="38" t="s">
         <v>93</v>
       </c>
       <c r="M27" s="18"/>
-      <c r="N27" s="23" t="s">
-        <v>45</v>
+      <c r="N27" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P27" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q27" s="18"/>
       <c r="R27" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S27" s="23"/>
     </row>
@@ -3747,83 +3785,83 @@
       <c r="K28" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L28" s="38" t="s">
-        <v>169</v>
+      <c r="L28" s="40" t="s">
+        <v>50</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="21"/>
       <c r="O28" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P28" s="21"/>
       <c r="Q28" s="16"/>
       <c r="R28" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S28" s="21"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>115</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="K29" s="25" t="s">
-        <v>146</v>
+      <c r="K29" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="L29" s="23"/>
       <c r="M29" s="18"/>
       <c r="N29" s="23"/>
       <c r="O29" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P29" s="23"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S29" s="23"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>108</v>
@@ -3835,93 +3873,93 @@
         <v>82</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="L30" s="38" t="s">
-        <v>180</v>
+      <c r="L30" s="37" t="s">
+        <v>103</v>
       </c>
       <c r="M30" s="16"/>
-      <c r="N30" s="21" t="s">
-        <v>45</v>
+      <c r="N30" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O30" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P30" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q30" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R30" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S30" s="21"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="D31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L31" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M31" s="18"/>
       <c r="N31" s="23"/>
       <c r="O31" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P31" s="23"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S31" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>101</v>
@@ -3947,30 +3985,30 @@
       <c r="M32" s="16"/>
       <c r="N32" s="21"/>
       <c r="O32" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P32" s="21"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S32" s="21"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>108</v>
@@ -3982,39 +4020,39 @@
         <v>92</v>
       </c>
       <c r="I33" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J33" s="18"/>
-      <c r="K33" s="25" t="s">
-        <v>103</v>
+      <c r="K33" s="41" t="s">
+        <v>93</v>
       </c>
       <c r="L33" s="23"/>
       <c r="M33" s="18"/>
       <c r="N33" s="23"/>
       <c r="O33" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P33" s="23"/>
       <c r="Q33" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R33" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S33" s="23"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="16" t="s">
@@ -4027,37 +4065,37 @@
         <v>92</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J34" s="16"/>
       <c r="K34" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="16"/>
       <c r="N34" s="21"/>
       <c r="O34" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P34" s="21"/>
       <c r="Q34" s="16"/>
       <c r="R34" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S34" s="21"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="18" t="s">
@@ -4070,7 +4108,7 @@
         <v>82</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J35" s="18"/>
       <c r="K35" s="23"/>
@@ -4078,7 +4116,7 @@
       <c r="M35" s="18"/>
       <c r="N35" s="23"/>
       <c r="O35" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P35" s="23"/>
       <c r="Q35" s="18"/>
@@ -4087,16 +4125,16 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="16" t="s">
@@ -4109,46 +4147,46 @@
         <v>152</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L36" s="38" t="s">
+      <c r="L36" s="37" t="s">
         <v>68</v>
       </c>
       <c r="M36" s="16"/>
-      <c r="N36" s="21" t="s">
-        <v>45</v>
+      <c r="N36" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O36" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q36" s="16"/>
       <c r="R36" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S36" s="21"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>108</v>
@@ -4163,88 +4201,88 @@
         <v>93</v>
       </c>
       <c r="J37" s="18"/>
-      <c r="K37" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L37" s="23" t="s">
-        <v>45</v>
+      <c r="K37" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="L37" s="41" t="s">
+        <v>116</v>
       </c>
       <c r="M37" s="18"/>
       <c r="N37" s="23"/>
       <c r="O37" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P37" s="23"/>
       <c r="Q37" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R37" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S37" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="16" t="s">
         <v>108</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>115</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="J38" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="J38" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="K38" s="24" t="s">
-        <v>146</v>
+      <c r="K38" s="40" t="s">
+        <v>68</v>
       </c>
       <c r="L38" s="21"/>
       <c r="M38" s="16"/>
       <c r="N38" s="21"/>
       <c r="O38" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P38" s="21"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S38" s="21"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>108</v>
@@ -4259,92 +4297,92 @@
         <v>68</v>
       </c>
       <c r="J39" s="18"/>
-      <c r="K39" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L39" s="23" t="s">
-        <v>45</v>
+      <c r="K39" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="L39" s="41" t="s">
+        <v>214</v>
       </c>
       <c r="M39" s="18"/>
-      <c r="N39" s="23" t="s">
-        <v>45</v>
+      <c r="N39" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O39" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P39" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q39" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R39" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S39" s="23"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="C40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>108</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H40" s="26" t="s">
         <v>92</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="16"/>
       <c r="N40" s="21"/>
       <c r="O40" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P40" s="21"/>
       <c r="Q40" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S40" s="21"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>155</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>108</v>
@@ -4358,40 +4396,40 @@
       <c r="I41" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J41" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="K41" s="23" t="s">
-        <v>45</v>
+      <c r="J41" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="K41" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="L41" s="23"/>
       <c r="M41" s="18"/>
       <c r="N41" s="23"/>
       <c r="O41" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P41" s="23"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S41" s="23"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>229</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>108</v>
@@ -4405,48 +4443,48 @@
       <c r="I42" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J42" s="36" t="s">
+      <c r="J42" s="35" t="s">
         <v>93</v>
       </c>
       <c r="K42" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="L42" s="21" t="s">
-        <v>45</v>
+      <c r="L42" s="40" t="s">
+        <v>214</v>
       </c>
       <c r="M42" s="16"/>
       <c r="N42" s="21"/>
       <c r="O42" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P42" s="21"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S42" s="21"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H43" s="26" t="s">
         <v>115</v>
@@ -4454,42 +4492,42 @@
       <c r="I43" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J43" s="34" t="s">
+      <c r="J43" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L43" s="39" t="s">
-        <v>51</v>
+      <c r="K43" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="L43" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="M43" s="18"/>
       <c r="N43" s="23"/>
       <c r="O43" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P43" s="23"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S43" s="23"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>108</v>
@@ -4501,7 +4539,7 @@
         <v>92</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J44" s="16"/>
       <c r="K44" s="24" t="s">
@@ -4511,81 +4549,81 @@
       <c r="M44" s="16"/>
       <c r="N44" s="21"/>
       <c r="O44" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P44" s="21"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S44" s="21"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>155</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H45" s="26" t="s">
         <v>92</v>
       </c>
       <c r="I45" s="20" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J45" s="18"/>
       <c r="K45" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L45" s="39" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="L45" s="38" t="s">
+        <v>116</v>
       </c>
       <c r="M45" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="N45" s="23"/>
       <c r="O45" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P45" s="23"/>
       <c r="Q45" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R45" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S45" s="23"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>108</v>
@@ -4601,80 +4639,80 @@
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="24" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="16"/>
       <c r="N46" s="21"/>
       <c r="O46" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P46" s="21"/>
       <c r="Q46" s="16"/>
       <c r="R46" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S46" s="21"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="18" t="s">
         <v>108</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H47" s="19" t="s">
         <v>115</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J47" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="K47" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L47" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="K47" s="41" t="s">
         <v>103</v>
+      </c>
+      <c r="L47" s="41" t="s">
+        <v>200</v>
       </c>
       <c r="M47" s="18"/>
       <c r="N47" s="23"/>
       <c r="O47" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P47" s="23"/>
       <c r="Q47" s="18"/>
       <c r="R47" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S47" s="23"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="16" t="s">
@@ -4687,40 +4725,40 @@
         <v>92</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J48" s="16"/>
       <c r="K48" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="16"/>
       <c r="N48" s="21"/>
       <c r="O48" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P48" s="21"/>
       <c r="Q48" s="16"/>
       <c r="R48" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S48" s="21"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>108</v>
@@ -4734,44 +4772,44 @@
       <c r="I49" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J49" s="37" t="s">
-        <v>51</v>
+      <c r="J49" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="K49" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="L49" s="39" t="s">
+      <c r="L49" s="38" t="s">
         <v>93</v>
       </c>
       <c r="M49" s="18"/>
       <c r="N49" s="23"/>
       <c r="O49" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P49" s="23"/>
       <c r="Q49" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R49" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S49" s="23"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="C50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="F50" s="16" t="s">
         <v>108</v>
@@ -4780,38 +4818,38 @@
         <v>66</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J50" s="33" t="s">
-        <v>169</v>
+        <v>50</v>
+      </c>
+      <c r="J50" s="32" t="s">
+        <v>266</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L50" s="38" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="L50" s="37" t="s">
+        <v>116</v>
       </c>
       <c r="M50" s="16"/>
-      <c r="N50" s="21" t="s">
-        <v>45</v>
+      <c r="N50" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O50" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q50" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R50" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S50" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4825,10 +4863,10 @@
         <v>39</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>269</v>
@@ -4873,13 +4911,13 @@
         <v>269</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J52" s="16"/>
       <c r="K52" s="24" t="s">
@@ -4887,16 +4925,16 @@
       </c>
       <c r="L52" s="21"/>
       <c r="M52" s="16"/>
-      <c r="N52" s="21" t="s">
-        <v>45</v>
+      <c r="N52" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P52" s="21"/>
       <c r="Q52" s="16"/>
       <c r="R52" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S52" s="21"/>
     </row>
@@ -4923,36 +4961,36 @@
         <v>280</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I53" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J53" s="37" t="s">
+      <c r="J53" s="36" t="s">
         <v>93</v>
       </c>
       <c r="K53" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="L53" s="39" t="s">
-        <v>202</v>
+      <c r="L53" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="M53" s="18"/>
-      <c r="N53" s="23" t="s">
-        <v>45</v>
+      <c r="N53" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O53" s="23"/>
       <c r="P53" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q53" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R53" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S53" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.35">
@@ -4973,13 +5011,13 @@
         <v>269</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J54" s="16"/>
       <c r="K54" s="24" t="s">
@@ -4987,14 +5025,14 @@
       </c>
       <c r="L54" s="21"/>
       <c r="M54" s="16"/>
-      <c r="N54" s="21" t="s">
-        <v>45</v>
+      <c r="N54" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O54" s="21"/>
       <c r="P54" s="21"/>
       <c r="Q54" s="16"/>
       <c r="R54" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S54" s="21"/>
     </row>
@@ -5024,13 +5062,13 @@
         <v>92</v>
       </c>
       <c r="I55" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J55" s="34" t="s">
-        <v>253</v>
+        <v>50</v>
+      </c>
+      <c r="J55" s="33" t="s">
+        <v>252</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L55" s="23"/>
       <c r="M55" s="18"/>
@@ -5039,10 +5077,10 @@
       <c r="P55" s="23"/>
       <c r="Q55" s="18"/>
       <c r="R55" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S55" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.35">
@@ -5077,14 +5115,14 @@
       <c r="K56" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="L56" s="38" t="s">
+      <c r="L56" s="37" t="s">
         <v>93</v>
       </c>
       <c r="M56" s="16"/>
       <c r="N56" s="21"/>
       <c r="O56" s="21"/>
       <c r="P56" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q56" s="16"/>
       <c r="R56" s="21"/>
@@ -5118,17 +5156,17 @@
       </c>
       <c r="J57" s="18"/>
       <c r="K57" s="23"/>
-      <c r="L57" s="39" t="s">
+      <c r="L57" s="38" t="s">
         <v>94</v>
       </c>
       <c r="M57" s="18"/>
       <c r="N57" s="23"/>
       <c r="O57" s="23"/>
       <c r="P57" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q57" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R57" s="23"/>
       <c r="S57" s="23"/>
@@ -5172,7 +5210,7 @@
       <c r="P58" s="21"/>
       <c r="Q58" s="16"/>
       <c r="R58" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S58" s="21"/>
     </row>
@@ -5190,7 +5228,7 @@
         <v>307</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F59" s="18" t="s">
         <v>269</v>
@@ -5202,33 +5240,35 @@
         <v>92</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="J59" s="18"/>
+        <v>266</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="K59" s="25" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L59" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M59" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N59" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N59" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O59" s="23"/>
       <c r="P59" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q59" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R59" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S59" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.35">
@@ -5251,10 +5291,10 @@
         <v>269</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I60" s="16"/>
       <c r="J60" s="16"/>
@@ -5294,10 +5334,10 @@
         <v>92</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="J61" s="34" t="s">
-        <v>51</v>
+        <v>116</v>
+      </c>
+      <c r="J61" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="K61" s="25" t="s">
         <v>93</v>
@@ -5308,13 +5348,13 @@
       <c r="O61" s="23"/>
       <c r="P61" s="23"/>
       <c r="Q61" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R61" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S61" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.35">
@@ -5372,35 +5412,35 @@
         <v>269</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>115</v>
       </c>
       <c r="I63" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J63" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="J63" s="33" t="s">
         <v>94</v>
       </c>
       <c r="K63" s="25" t="s">
         <v>93</v>
       </c>
       <c r="L63" s="23"/>
-      <c r="M63" s="34" t="s">
+      <c r="M63" s="33" t="s">
         <v>93</v>
       </c>
       <c r="N63" s="23"/>
       <c r="O63" s="23"/>
       <c r="P63" s="23"/>
       <c r="Q63" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R63" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S63" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.35">
@@ -5417,7 +5457,7 @@
         <v>269</v>
       </c>
       <c r="G64" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H64" s="31" t="s">
         <v>115</v>
@@ -5430,14 +5470,14 @@
       <c r="N64" s="23"/>
       <c r="O64" s="23"/>
       <c r="P64" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q64" s="18"/>
       <c r="R64" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S64" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
@@ -5448,7 +5488,7 @@
         <v>327</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>328</v>
@@ -5460,37 +5500,37 @@
         <v>269</v>
       </c>
       <c r="G65" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K65" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L65" s="23" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="L65" s="41" t="s">
+        <v>116</v>
       </c>
       <c r="M65" s="23"/>
-      <c r="N65" s="23" t="s">
-        <v>45</v>
+      <c r="N65" s="46" t="s">
+        <v>50</v>
       </c>
       <c r="O65" s="23"/>
       <c r="P65" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q65" s="18"/>
       <c r="R65" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S65" s="23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.35">
@@ -5519,31 +5559,31 @@
         <v>67</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J66" s="16"/>
       <c r="K66" s="21"/>
-      <c r="L66" s="38" t="s">
-        <v>146</v>
+      <c r="L66" s="37" t="s">
+        <v>214</v>
       </c>
       <c r="M66" s="16"/>
-      <c r="N66" s="21" t="s">
-        <v>45</v>
+      <c r="N66" s="45" t="s">
+        <v>50</v>
       </c>
       <c r="O66" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P66" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q66" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R66" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S66" s="21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.35">
@@ -5566,35 +5606,35 @@
         <v>82</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" s="35" t="s">
-        <v>253</v>
+        <v>58</v>
+      </c>
+      <c r="J67" s="34" t="s">
+        <v>252</v>
       </c>
       <c r="K67" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L67" s="33" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="L67" s="32" t="s">
+        <v>116</v>
       </c>
       <c r="M67" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N67" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N67" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O67" s="16"/>
       <c r="P67" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q67" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R67" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.35">
@@ -5605,7 +5645,7 @@
         <v>335</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6" t="s">
@@ -5617,37 +5657,37 @@
       <c r="G68" s="18"/>
       <c r="H68" s="19"/>
       <c r="I68" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J68" s="37" t="s">
-        <v>180</v>
+        <v>50</v>
+      </c>
+      <c r="J68" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="K68" s="20" t="s">
         <v>68</v>
       </c>
       <c r="L68" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="M68" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M68" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="N68" s="18" t="s">
-        <v>45</v>
+      <c r="N68" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O68" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P68" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q68" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R68" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S68" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.35">
@@ -5672,35 +5712,35 @@
       <c r="I69" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J69" s="33" t="s">
-        <v>202</v>
+      <c r="J69" s="32" t="s">
+        <v>200</v>
       </c>
       <c r="K69" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="L69" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="M69" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="N69" s="16" t="s">
-        <v>45</v>
+      <c r="L69" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="M69" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="N69" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O69" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P69" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q69" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R69" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S69" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.35">
@@ -5723,37 +5763,37 @@
       <c r="G70" s="18"/>
       <c r="H70" s="19"/>
       <c r="I70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M70" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N70" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S70" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.35">
@@ -5768,7 +5808,7 @@
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F71" s="16" t="s">
         <v>337</v>
@@ -5776,37 +5816,37 @@
       <c r="G71" s="16"/>
       <c r="H71" s="17"/>
       <c r="I71" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J71" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="J71" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K71" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L71" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="M71" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="K71" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L71" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="M71" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="N71" s="16" t="s">
-        <v>45</v>
+      <c r="N71" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O71" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P71" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q71" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R71" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S71" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.35">
@@ -5817,7 +5857,7 @@
         <v>348</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="6" t="s">
@@ -5829,37 +5869,37 @@
       <c r="G72" s="18"/>
       <c r="H72" s="19"/>
       <c r="I72" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="J72" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J72" s="36" t="s">
         <v>68</v>
       </c>
       <c r="K72" s="20" t="s">
         <v>93</v>
       </c>
       <c r="L72" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="M72" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M72" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="N72" s="18" t="s">
-        <v>45</v>
+      <c r="N72" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O72" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P72" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q72" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R72" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S72" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.35">
@@ -5882,51 +5922,51 @@
       <c r="G73" s="16"/>
       <c r="H73" s="17"/>
       <c r="I73" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J73" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="J73" s="35" t="s">
         <v>68</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L73" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="M73" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="L73" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="M73" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="N73" s="16" t="s">
-        <v>45</v>
+      <c r="N73" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O73" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P73" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q73" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R73" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="18" t="s">
@@ -5937,50 +5977,50 @@
       <c r="I74" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J74" s="34" t="s">
-        <v>202</v>
+      <c r="J74" s="33" t="s">
+        <v>200</v>
       </c>
       <c r="K74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M74" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N74" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S74" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F75" s="16" t="s">
         <v>337</v>
@@ -5988,51 +6028,51 @@
       <c r="G75" s="16"/>
       <c r="H75" s="17"/>
       <c r="I75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M75" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N75" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S75" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E76" s="6"/>
       <c r="F76" s="18" t="s">
@@ -6041,51 +6081,51 @@
       <c r="G76" s="18"/>
       <c r="H76" s="19"/>
       <c r="I76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M76" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N76" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S76" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>101</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="16" t="s">
@@ -6094,52 +6134,52 @@
       <c r="G77" s="16"/>
       <c r="H77" s="17"/>
       <c r="I77" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J77" s="33" t="s">
-        <v>202</v>
+        <v>58</v>
+      </c>
+      <c r="J77" s="32" t="s">
+        <v>200</v>
       </c>
       <c r="K77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M77" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N77" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S77" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>337</v>
@@ -6147,52 +6187,52 @@
       <c r="G78" s="18"/>
       <c r="H78" s="19"/>
       <c r="I78" s="20" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K78" s="20" t="s">
         <v>93</v>
       </c>
       <c r="L78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M78" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N78" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S78" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>306</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F79" s="16" t="s">
         <v>337</v>
@@ -6200,52 +6240,52 @@
       <c r="G79" s="16"/>
       <c r="H79" s="17"/>
       <c r="I79" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="J79" s="33" t="s">
-        <v>146</v>
+        <v>214</v>
+      </c>
+      <c r="J79" s="32" t="s">
+        <v>214</v>
       </c>
       <c r="K79" s="22" t="s">
         <v>68</v>
       </c>
       <c r="L79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M79" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N79" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>337</v>
@@ -6253,52 +6293,52 @@
       <c r="G80" s="18"/>
       <c r="H80" s="19"/>
       <c r="I80" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K80" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="L80" s="18" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="L80" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="M80" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N80" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="O80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S80" s="18" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F81" s="16" t="s">
         <v>337</v>
@@ -6309,52 +6349,52 @@
         <v>93</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K81" s="22" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="N81" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="Q81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="R81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="S81" s="16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B86" s="29" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.35">
@@ -6362,26 +6402,26 @@
         <v>44</v>
       </c>
       <c r="B87" s="29" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" s="29" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B88" s="29" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" s="29" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -6406,6 +6446,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100099975770C1F1147804C2B8EA59B7744" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="449a151c82d64f5fb2f07b6eeab9cc56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ff4e4123-c072-43f7-8ca2-317c8e6eca2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee3512447ab763bfc9d78f4694d5743c" ns2:_="">
     <xsd:import namespace="ff4e4123-c072-43f7-8ca2-317c8e6eca2e"/>
@@ -6537,23 +6592,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8147BA37-0A84-40D1-B6E1-3ABF3F96C592}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B176E064-9437-41A8-B561-BD64CA049106}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff4e4123-c072-43f7-8ca2-317c8e6eca2e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70BBA54C-6A36-4007-821A-D5947083342F}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10148454-9C33-4BA1-B41D-6C8C69228E1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -6568,28 +6632,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{061ED646-E56B-4D2A-92F6-EE2181C58515}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{746145FF-1B78-49B7-89C8-C55EEF002280}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff4e4123-c072-43f7-8ca2-317c8e6eca2e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>